<commit_message>
Beginnings of documentations for Elex format
</commit_message>
<xml_diff>
--- a/fielddescriptions.xlsx
+++ b/fielddescriptions.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{6B46DF32-5C05-488C-A1B0-41430B5314BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -144,14 +144,85 @@
   </si>
   <si>
     <t>winner</t>
+  </si>
+  <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unique race ID for a specific state</t>
+  </si>
+  <si>
+    <t>Character string indicating the type of race (for example, GOP Primary, General, Democratic Caucus)</t>
+  </si>
+  <si>
+    <t>Single-character race type ID D (Dem Primary), R (GOP Primary), G (General), E (Dem Caucus), S (GOP Caucus)</t>
+  </si>
+  <si>
+    <t>? In practice, raceid and delimiter and reportingunitid</t>
+  </si>
+  <si>
+    <t>AP-assigned unique ID for this candidate in a state's race. If a candidate is running in multiple races, this candidate has a different candidateid in each race</t>
+  </si>
+  <si>
+    <t>Description of the office, ballot initiative or other (if applicable)</t>
+  </si>
+  <si>
+    <t>Ballot order of this candidate. There may be gaps in sequence in this order field.</t>
+  </si>
+  <si>
+    <t>For presidential primaries, delegates won by this candidate in this district</t>
+  </si>
+  <si>
+    <t>In a general election in a presidential year, the state or U.S. national electoral count</t>
+  </si>
+  <si>
+    <t>In a general election in a presidential year, the candidate's electoral votes</t>
+  </si>
+  <si>
+    <t>County FIPS code, a geographical standard that allows data to be matched</t>
+  </si>
+  <si>
+    <t>Candidate's first name</t>
+  </si>
+  <si>
+    <t>A flag that indicates the candidate is an incumbent. In Elex CSV format, this is TRUE or FALSE</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Candidate's last name</t>
+  </si>
+  <si>
+    <t>Date of the election day, in format m/d/yyyy</t>
+  </si>
+  <si>
+    <t>Time last updated. Sample: 2018-03-07T17:24:47.600Z</t>
+  </si>
+  <si>
+    <t>Region the vote results are reported from: "national" for presidential results and electoral count at the U.S. national rolled-up summary level (only for the general election in a presidential year); "state" for state-level results; "subunit" for results at the RU or FIPS code level; "district" for delegate results at the district level from the presidential primaries or presidential results and electoral counts by district (currently, in Maine and Nebraska) for the general election in a presidential year</t>
+  </si>
+  <si>
+    <t>Indicates that the race is national. "TRUE"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,8 +250,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,138 +567,289 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95467A3-01C8-4854-BF8E-398751EB7672}">
-  <dimension ref="A1:AN1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FAB618-7688-4A0E-8FF4-867B22C49E77}">
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>